<commit_message>
working for almost all maps
Converted all shapefiles to WGS 84, EPSG 4269
HEE and HUD fail due to incorrect number of stations.
</commit_message>
<xml_diff>
--- a/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_ACE_2020.xlsx
+++ b/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_ACE_2020.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t>Flags</t>
   </si>
@@ -376,6 +376,30 @@
   </si>
   <si>
     <t xml:space="preserve">2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Res_Bounding_Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK_Bounding_Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Station_Map_Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK_WQ_Map_Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK_MET_Map_Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK_NUT_Map_Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
   </si>
   <si>
     <t xml:space="preserve">Options</t>
@@ -1439,99 +1463,107 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-80.739900000000006</v>
+        <v>-80.7155</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>-80.739900000000006</v>
+        <v>-80.6925</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>32.770499999999998</v>
+        <v>32.2987</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>32.770499999999998</v>
+        <v>32.318</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-80.150800000000004</v>
+        <v>-80.1588</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>-80.150800000000004</v>
+        <v>-80.1818</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="E4"/>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>32.328299999999999</v>
+        <v>32.7158</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>32.328299999999999</v>
+        <v>32.6965</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="E5"/>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6"/>
+      <c r="B6"/>
       <c r="C6" t="s">
-        <v>73</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1554,98 +1586,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1693,402 +1725,402 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E2"/>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D4" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E5"/>
       <c r="F5" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="E6"/>
       <c r="F6" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" t="s">
         <v>148</v>
       </c>
-      <c r="C8" t="s">
-        <v>140</v>
-      </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E8"/>
       <c r="F8" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" t="s">
         <v>149</v>
-      </c>
-      <c r="B9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D9" t="s">
-        <v>141</v>
       </c>
       <c r="E9"/>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" t="s">
         <v>148</v>
       </c>
-      <c r="C10" t="s">
-        <v>140</v>
-      </c>
       <c r="D10" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E10"/>
       <c r="F10" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" t="s">
         <v>148</v>
       </c>
-      <c r="C11" t="s">
-        <v>140</v>
-      </c>
       <c r="D11" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" t="s">
         <v>148</v>
       </c>
-      <c r="C12" t="s">
-        <v>140</v>
-      </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E12"/>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E13"/>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E14"/>
       <c r="F14" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D15" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E15"/>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E16"/>
       <c r="F16" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E18"/>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E19"/>
       <c r="F19" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C20" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E21"/>
       <c r="F21" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C22" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D22" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E22"/>
       <c r="F22" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed (mostly) aspect ratio issues
</commit_message>
<xml_diff>
--- a/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_ACE_2020.xlsx
+++ b/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_ACE_2020.xlsx
@@ -1483,10 +1483,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-80.7155</v>
+        <v>-80.8442</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>-80.6925</v>
+        <v>-80.7652</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -1503,10 +1503,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>32.2987</v>
+        <v>32.1791</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>32.318</v>
+        <v>32.2458</v>
       </c>
       <c r="C3" t="s">
         <v>125</v>
@@ -1521,10 +1521,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-80.1588</v>
+        <v>-80.051</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>-80.1818</v>
+        <v>-80.1309</v>
       </c>
       <c r="C4" t="s">
         <v>125</v>
@@ -1539,10 +1539,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>32.7158</v>
+        <v>32.8437</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>32.6965</v>
+        <v>32.7773</v>
       </c>
       <c r="C5" t="s">
         <v>125</v>

</xml_diff>